<commit_message>
#8 - Serial content
</commit_message>
<xml_diff>
--- a/2.Design/Template/Bieu_mau_nhap_hang.xlsx
+++ b/2.Design/Template/Bieu_mau_nhap_hang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2.DoanLV4_Document\LogDez\1.Document\WMS_Documents\2.Design\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\WMS\WMS_Documents\2.Design\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE24CBF-4C28-4BAF-88FE-023A06FE6782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F72C2CB-60CE-441C-90D5-FC9E74FF43BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tên hàng</t>
   </si>
@@ -120,6 +120,9 @@
       </rPr>
       <t>(dd/MM/yyyy)</t>
     </r>
+  </si>
+  <si>
+    <t>Nguồn gốc</t>
   </si>
 </sst>
 </file>
@@ -525,27 +528,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -575,6 +579,9 @@
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>